<commit_message>
Updated xlbean version to v0.3.0
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/xlscript/Test_toBean.xlsx
+++ b/src/test/resources/org/xlbean/xlscript/Test_toBean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\xldsl\xlscript\src\test\resources\org\xlbean\xlscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C6268-14FF-4886-8065-AE67293ECAEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9619E53E-7E09-4932-A103-6E0E921CD368}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="1044" windowWidth="21948" windowHeight="12660" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
+    <workbookView xWindow="6252" yWindow="3684" windowWidth="21948" windowHeight="12660" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
   </bookViews>
   <sheets>
     <sheet name="toBean" sheetId="3" r:id="rId1"/>
@@ -76,7 +76,8 @@
     <t>list#key?toMap=key</t>
   </si>
   <si>
-    <t>list#value?toMap=value&amp;type=string</t>
+    <t>list#value?toMap=value&amp;readAs=text</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -440,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810AB0D9-B152-49D3-81E8-A5F04E8D5F3D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -466,46 +467,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>